<commit_message>
Updated code with action center changes
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheolmin.hwang\Documents\UiPath\SunWest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SMWC\github\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IdentifiedCat" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Category_C" sheetId="4" r:id="rId5"/>
     <sheet name="Category_D" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -374,12 +374,15 @@
   </si>
   <si>
     <t>passwd2</t>
+  </si>
+  <si>
+    <t>A99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -721,22 +724,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -751,18 +754,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,7 +776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -788,7 +791,7 @@
         <v>C01 - Document Received</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -803,7 +806,7 @@
         <v>C02 - Question Related to an unknown condition</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -818,7 +821,7 @@
         <v>C03 - Question Related to an known condition</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -833,7 +836,7 @@
         <v>C04 - Question on unknown Condition Resolution ETA</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>72</v>
       </c>
@@ -848,7 +851,7 @@
         <v>C05a - Qusetion on known Condition Resolution ETA</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>73</v>
       </c>
@@ -863,7 +866,7 @@
         <v>C05b - Question on CD ETA</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
@@ -878,7 +881,7 @@
         <v>C06a - Question about Docs ETA</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -893,7 +896,7 @@
         <v>C06b - Question on Loan Status</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
@@ -908,7 +911,7 @@
         <v>C07 - Question on Payment Status</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>50</v>
       </c>
@@ -923,7 +926,7 @@
         <v>C08 - Question on Other</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
@@ -938,7 +941,7 @@
         <v>C09 - Response related to a Condition</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>54</v>
       </c>
@@ -953,7 +956,7 @@
         <v>C10 - Request for CTC</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
@@ -968,7 +971,7 @@
         <v>C11 - Request to esclalate CD</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
@@ -983,7 +986,7 @@
         <v>C12 - Request to provide Document</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>C13 - Request to Update Data</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>C14 - Request Other</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>C15 - Manual Queue</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>66</v>
       </c>
@@ -1043,7 +1046,7 @@
         <v>C16 - Manual Queue for TAT</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>C17 - Urgent Queue</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>C18 - Get Loan Number Queue</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>C19 - Request Password Queue</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
@@ -1111,20 +1114,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>A01 - Download and Upload Attachments</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>82</v>
       </c>
@@ -1157,11 +1160,11 @@
       </c>
       <c r="C3" s="4"/>
       <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F13" si="0">CONCATENATE(A3," - ",B3)</f>
+        <f t="shared" ref="F3:F14" si="0">CONCATENATE(A3," - ",B3)</f>
         <v>A02 - Download and Uplaod Attachments (PP)</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>A02a - Send to sysadmin for decryption</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>86</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>E01 - Send standard acknowledgment (no ETA)</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>88</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>E02 - Send acknowledgment with ETA</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>90</v>
       </c>
@@ -1213,7 +1216,7 @@
         <v>E03 - Respond to sender (Template)</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>L01 - Document Link Processing</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>94</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>L01a - Document Processing for Zix</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>96</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>L01b - Document Processing for Outlook</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>98</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>L01c - Document Processing for Qualia</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>100</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>L01d - Document Processing for DHI Title</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>102</v>
       </c>
@@ -1289,6 +1292,18 @@
       <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>L01e - Document Processing for Citrix</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>A99 - No Action Required</v>
       </c>
     </row>
   </sheetData>
@@ -1305,13 +1320,13 @@
       <selection activeCell="A4" sqref="A4:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -1322,7 +1337,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>111</v>
       </c>
@@ -1333,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>113</v>
       </c>
@@ -1362,12 +1377,12 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1378,7 +1393,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1389,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1411,7 +1426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1422,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1447,12 +1462,12 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1463,7 +1478,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1474,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1485,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1496,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1507,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>

</xml_diff>